<commit_message>
fechas formateadas y corregido bug cuando solo hay un activo
</commit_message>
<xml_diff>
--- a/rem-web/src/main/webapp/plantillas/plugin/Propuesta_alquileres_bankia/PROPUESTA_BANKIA.xlsx
+++ b/rem-web/src/main/webapp/plantillas/plugin/Propuesta_alquileres_bankia/PROPUESTA_BANKIA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Acta Comité " sheetId="1" state="visible" r:id="rId2"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
-  <si>
-    <t xml:space="preserve">Algo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t xml:space="preserve">PROPUESTAS DE ALQUILER PRESENTADAS AL COMITÉ DE DOBLE FIRMA DE FECHA 09/04/2017</t>
   </si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">RESOLUCIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
     <t xml:space="preserve">PROPUESTA DE OFERTA COMERCIAL A COMITÉ</t>
@@ -851,35 +845,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A2:U7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="6" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.9797570850202"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4008097165992"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0607287449393"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6477732793522"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.7975708502024"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.4412955465587"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.1093117408907"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.5101214574899"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="N2" s="2"/>
     </row>
@@ -908,67 +907,67 @@
     </row>
     <row r="5" s="5" customFormat="true" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="U5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,9 +994,7 @@
       <c r="U6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1037,26 +1034,26 @@
   </sheetPr>
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B106" activeCellId="0" sqref="B106"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="46.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="68.1295546558705"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="8" width="11.5708502024291"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="12"/>
     </row>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="14"/>
     </row>
@@ -1080,39 +1077,39 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="23"/>
     </row>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="27"/>
     </row>
@@ -1140,7 +1137,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="29"/>
     </row>
@@ -1150,19 +1147,19 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="19"/>
     </row>
@@ -1172,7 +1169,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="29"/>
     </row>
@@ -1182,7 +1179,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="30"/>
     </row>
@@ -1192,25 +1189,25 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="30"/>
     </row>
@@ -1224,7 +1221,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" s="33"/>
     </row>
@@ -1238,31 +1235,31 @@
     </row>
     <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="36"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="36"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="37"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="38"/>
     </row>
@@ -1276,7 +1273,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="33"/>
     </row>
@@ -1290,31 +1287,31 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" s="29"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="30"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="30"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="39"/>
     </row>
@@ -1328,7 +1325,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B54" s="27"/>
     </row>
@@ -1342,31 +1339,31 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="40"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="41"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" s="41"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="42" t="e">
         <f aca="false">(B57*12)/B37</f>
@@ -1375,7 +1372,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="43" t="e">
         <f aca="false">B61-B63</f>
@@ -1384,7 +1381,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63" s="43"/>
     </row>
@@ -1394,10 +1391,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,55 +1403,55 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B67" s="39"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B68" s="39"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B69" s="39"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B70" s="39"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B71" s="39"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B72" s="39"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="39"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B74" s="39"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B75" s="39"/>
     </row>
@@ -1468,7 +1465,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B78" s="27"/>
     </row>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B88" s="27"/>
     </row>
@@ -1524,7 +1521,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B91" s="50"/>
     </row>
@@ -1544,9 +1541,9 @@
       <c r="B94" s="51"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="52" t="str">
-        <f aca="false">CONCATENATE("1. Renta ",B106," €/mes. Bonificada a ",B106," €/mes")</f>
-        <v>1. Renta  €/mes. Bonificada a  €/mes</v>
+      <c r="A95" s="52" t="e">
+        <f aca="false">CONCATENATE("1. Renta ",B61," €/mes. Bonificada a ",B62," €/mes")</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="B95" s="52"/>
     </row>
@@ -1559,26 +1556,26 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="54" t="str">
-        <f aca="false">CONCATENATE("3. ",B106," mes de carencia por suministros")</f>
+        <f aca="false">CONCATENATE("3. ",B60," mes de carencia por suministros")</f>
         <v>3.  mes de carencia por suministros</v>
       </c>
       <c r="B97" s="54"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="50" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B98" s="50"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="50" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B99" s="50"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B100" s="50"/>
     </row>

</xml_diff>